<commit_message>
(REBUILD) - The structure of the projects area     * The data now comes from a projects.json, which can be generated from an Excel sheet using the python projectsXLSX_to_json_converter.py script.     * Created a ReadMe_coversion_workflow file - Refactoring index.html     * JavaScript code removed from the structure and packed into separate topic-related files.
</commit_message>
<xml_diff>
--- a/src/data/data_conversion/files_to_convert/skills_json.xlsx
+++ b/src/data/data_conversion/files_to_convert/skills_json.xlsx
@@ -136,7 +136,7 @@
     <t>supportive &amp; training</t>
   </si>
   <si>
-    <t>TYPO3 Wordpress</t>
+    <t>Wordpress TYPO3</t>
   </si>
   <si>
     <t>TypoScript, Website modeling, Integrate own code, User management, Child themes</t>
@@ -145,10 +145,10 @@
     <t>Project Management</t>
   </si>
   <si>
-    <t>IPMA ICB4 Level D</t>
-  </si>
-  <si>
-    <t>Practice, People, Perspective</t>
+    <t>IPMA ICB4</t>
+  </si>
+  <si>
+    <t>Level D, Practice, People, Perspective</t>
   </si>
   <si>
     <t>Major customer vehicle delivery</t>
@@ -1745,7 +1745,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6562" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.5078" style="1" customWidth="1"/>
     <col min="4" max="9" width="16.3516" style="1" customWidth="1"/>
     <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
@@ -1954,7 +1955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="56.45" customHeight="1">
+    <row r="8" ht="46.7" customHeight="1">
       <c r="A8" t="s" s="21">
         <v>9</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="56.45" customHeight="1">
+    <row r="11" ht="42.6" customHeight="1">
       <c r="A11" t="s" s="21">
         <v>9</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" ht="79.45" customHeight="1">
+    <row r="35" ht="56.45" customHeight="1">
       <c r="A35" t="s" s="28">
         <v>9</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" ht="79.45" customHeight="1">
+    <row r="36" ht="42.6" customHeight="1">
       <c r="A36" t="s" s="21">
         <v>43</v>
       </c>

</xml_diff>